<commit_message>
Archivos cuaderno tema 11
Archivos tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/Escaleta_MA_06_08_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion08/Escaleta_MA_06_08_CO.xlsx
@@ -243,9 +243,6 @@
     <t>En la presentación colocar imágenes que rerpesenten situaciones que se representen con números decimales, por ejemplo, una competencia de natación oo atletismo. Precios. Cantidades en gramos o kilogramos, etc. En cada ficha dar la explicación del algoritmo correspondiente y mostrar el desarrollo de una situación. Además incluir si es posible las propiedades. Proponer practica.</t>
   </si>
   <si>
-    <t>Ejercicios de practica de adición y sustracción de números decimales</t>
-  </si>
-  <si>
     <t>En el motor aleatorio, seleccionar las opciones suma y resta (únicamente). Seleccionar nivel 2 en complejidad.</t>
   </si>
   <si>
@@ -306,12 +303,6 @@
     <t>Actividades sobre El redondeo de números decimales</t>
   </si>
   <si>
-    <t>Practica operaciones combinadas</t>
-  </si>
-  <si>
-    <t>Resuelve operaciones combinados con números decimales</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La adición y la sustracción de números decimales</t>
   </si>
   <si>
@@ -420,9 +411,6 @@
     <t>Actividad de práctica de la adición y la sustracción de números decimales</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para identificar las propiedades de la adición </t>
-  </si>
-  <si>
     <t>Dar ejemplos en los cuales se apliquen las propiedades de la adición de númerps decimales. Los estudiantes deberán identicar cuál es la propiedad que corresponde.</t>
   </si>
   <si>
@@ -498,9 +486,6 @@
     <t>Interactivo que resume aspectos básicos sobre las operaciones con números decimales</t>
   </si>
   <si>
-    <t>Resuelve problemas desarrollando operaciones combinadas</t>
-  </si>
-  <si>
     <t>Actividad para solucionar problemas con operaciones combinadas entre decimales</t>
   </si>
   <si>
@@ -535,6 +520,21 @@
   </si>
   <si>
     <t>Evalúa tus conocimientos sobre Las operaciones con números decimales</t>
+  </si>
+  <si>
+    <t>Actividad para identificar las propiedades de la adición de decimales</t>
+  </si>
+  <si>
+    <t>Ejercicios de práctica de adición y sustracción de números decimales</t>
+  </si>
+  <si>
+    <t>Practica operaciones combinadas con decimales</t>
+  </si>
+  <si>
+    <t>Resuelve operaciones combinadas con números decimales</t>
+  </si>
+  <si>
+    <t>Resuelve problemas mediante operaciones combinadas</t>
   </si>
 </sst>
 </file>
@@ -830,6 +830,15 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,15 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1214,82 +1214,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="44"/>
+      <c r="N1" s="47"/>
       <c r="O1" s="38" t="s">
         <v>27</v>
       </c>
       <c r="P1" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="40"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="44"/>
       <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1298,11 +1298,11 @@
       </c>
       <c r="O2" s="38"/>
       <c r="P2" s="38"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="50"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="39"/>
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
@@ -1316,12 +1316,12 @@
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
       <c r="G3" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>30</v>
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="W3" s="22"/>
     </row>
@@ -1376,12 +1376,12 @@
         <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="23"/>
       <c r="G4" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H4" s="24">
         <v>2</v>
@@ -1390,7 +1390,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>29</v>
@@ -1432,12 +1432,12 @@
         <v>49</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="23"/>
       <c r="G5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="11">
         <v>3</v>
@@ -1446,7 +1446,7 @@
         <v>30</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>30</v>
@@ -1459,7 +1459,7 @@
         <v>23</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="P5" s="17" t="s">
         <v>30</v>
@@ -1492,12 +1492,12 @@
         <v>49</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="23"/>
       <c r="G6" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H6" s="24">
         <v>4</v>
@@ -1506,7 +1506,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>30</v>
@@ -1519,7 +1519,7 @@
         <v>26</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>29</v>
@@ -1531,13 +1531,13 @@
         <v>35</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="W6" s="22"/>
     </row>
@@ -1552,12 +1552,12 @@
         <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="23"/>
       <c r="G7" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H7" s="11">
         <v>5</v>
@@ -1566,7 +1566,7 @@
         <v>30</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>29</v>
@@ -1608,12 +1608,12 @@
         <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="23"/>
       <c r="G8" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H8" s="24">
         <v>6</v>
@@ -1622,7 +1622,7 @@
         <v>30</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>30</v>
@@ -1635,7 +1635,7 @@
         <v>25</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P8" s="17" t="s">
         <v>29</v>
@@ -1668,14 +1668,14 @@
         <v>49</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H9" s="11">
         <v>7</v>
@@ -1684,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>29</v>
@@ -1705,13 +1705,13 @@
         <v>38</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T9" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="U9" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W9" s="22"/>
     </row>
@@ -1726,12 +1726,12 @@
         <v>49</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="23"/>
       <c r="G10" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="24">
         <v>8</v>
@@ -1740,7 +1740,7 @@
         <v>32</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>30</v>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P10" s="17" t="s">
         <v>29</v>
@@ -1768,10 +1768,10 @@
         <v>34</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="W10" s="22"/>
     </row>
@@ -1786,7 +1786,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="23"/>
@@ -1800,7 +1800,7 @@
         <v>30</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>29</v>
@@ -1842,7 +1842,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="23"/>
@@ -1856,7 +1856,7 @@
         <v>32</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>29</v>
@@ -1898,12 +1898,12 @@
         <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="23"/>
       <c r="G13" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="11">
         <v>11</v>
@@ -1912,7 +1912,7 @@
         <v>30</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>30</v>
@@ -1925,7 +1925,7 @@
         <v>25</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P13" s="17" t="s">
         <v>29</v>
@@ -1940,7 +1940,7 @@
         <v>36</v>
       </c>
       <c r="T13" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U13" s="20" t="s">
         <v>37</v>
@@ -1958,7 +1958,7 @@
         <v>49</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>31</v>
@@ -1974,7 +1974,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>29</v>
@@ -1995,13 +1995,13 @@
         <v>38</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="U14" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W14" s="22"/>
     </row>
@@ -2016,12 +2016,12 @@
         <v>49</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="23"/>
       <c r="G15" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="11">
         <v>13</v>
@@ -2030,7 +2030,7 @@
         <v>32</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>30</v>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P15" s="17" t="s">
         <v>29</v>
@@ -2058,10 +2058,10 @@
         <v>34</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U15" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="W15" s="22"/>
     </row>
@@ -2076,12 +2076,12 @@
         <v>49</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="23"/>
       <c r="G16" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H16" s="24">
         <v>14</v>
@@ -2090,7 +2090,7 @@
         <v>30</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>29</v>
@@ -2101,7 +2101,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P16" s="17" t="s">
         <v>29</v>
@@ -2134,12 +2134,12 @@
         <v>49</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="23"/>
       <c r="G17" s="27" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H17" s="11">
         <v>15</v>
@@ -2148,7 +2148,7 @@
         <v>30</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>30</v>
@@ -2161,7 +2161,7 @@
         <v>24</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>29</v>
@@ -2194,12 +2194,12 @@
         <v>49</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="23"/>
       <c r="G18" s="27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H18" s="24">
         <v>16</v>
@@ -2208,7 +2208,7 @@
         <v>30</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>29</v>
@@ -2250,12 +2250,12 @@
         <v>49</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="23"/>
       <c r="G19" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H19" s="11">
         <v>17</v>
@@ -2264,7 +2264,7 @@
         <v>32</v>
       </c>
       <c r="J19" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>29</v>
@@ -2275,7 +2275,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="17"/>
       <c r="O19" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P19" s="17" t="s">
         <v>30</v>
@@ -2308,14 +2308,14 @@
         <v>49</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H20" s="24">
         <v>18</v>
@@ -2324,7 +2324,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>29</v>
@@ -2345,13 +2345,13 @@
         <v>38</v>
       </c>
       <c r="S20" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="U20" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W20" s="22"/>
     </row>
@@ -2371,7 +2371,7 @@
       <c r="E21" s="26"/>
       <c r="F21" s="23"/>
       <c r="G21" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H21" s="11">
         <v>19</v>
@@ -2380,7 +2380,7 @@
         <v>30</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>30</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P21" s="17" t="s">
         <v>29</v>
@@ -2408,7 +2408,7 @@
         <v>36</v>
       </c>
       <c r="T21" s="21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="U21" s="20" t="s">
         <v>37</v>
@@ -2431,7 +2431,7 @@
       <c r="E22" s="26"/>
       <c r="F22" s="23"/>
       <c r="G22" s="27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H22" s="24">
         <v>20</v>
@@ -2440,7 +2440,7 @@
         <v>30</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>30</v>
@@ -2453,7 +2453,7 @@
         <v>25</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P22" s="17" t="s">
         <v>29</v>
@@ -2468,7 +2468,7 @@
         <v>36</v>
       </c>
       <c r="T22" s="21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U22" s="20" t="s">
         <v>37</v>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H23" s="11">
         <v>21</v>
@@ -2502,7 +2502,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K23" s="14" t="s">
         <v>29</v>
@@ -2526,7 +2526,7 @@
         <v>55</v>
       </c>
       <c r="T23" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="U23" s="20" t="s">
         <v>57</v>
@@ -2544,7 +2544,7 @@
         <v>49</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="23"/>
@@ -2558,7 +2558,7 @@
         <v>32</v>
       </c>
       <c r="J24" s="28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>29</v>
@@ -2600,12 +2600,12 @@
         <v>49</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="23"/>
       <c r="G25" s="27" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="H25" s="11">
         <v>23</v>
@@ -2614,7 +2614,7 @@
         <v>30</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>29</v>
@@ -2656,12 +2656,12 @@
         <v>49</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="23"/>
       <c r="G26" s="27" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="H26" s="24">
         <v>24</v>
@@ -2670,7 +2670,7 @@
         <v>30</v>
       </c>
       <c r="J26" s="28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K26" s="14" t="s">
         <v>29</v>
@@ -2712,7 +2712,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="23"/>
@@ -2726,7 +2726,7 @@
         <v>32</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>29</v>
@@ -2768,12 +2768,12 @@
         <v>49</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="23"/>
       <c r="G28" s="27" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="H28" s="24">
         <v>26</v>
@@ -2782,7 +2782,7 @@
         <v>30</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>29</v>
@@ -2793,7 +2793,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="17"/>
       <c r="O28" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P28" s="17" t="s">
         <v>29</v>
@@ -2826,12 +2826,12 @@
         <v>49</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="23"/>
       <c r="G29" s="27" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H29" s="11">
         <v>27</v>
@@ -2840,7 +2840,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K29" s="14" t="s">
         <v>29</v>
@@ -2851,7 +2851,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="17"/>
       <c r="O29" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="P29" s="17" t="s">
         <v>30</v>
@@ -2884,7 +2884,7 @@
         <v>49</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>31</v>
@@ -2900,7 +2900,7 @@
         <v>30</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>29</v>
@@ -2942,12 +2942,12 @@
         <v>49</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
       <c r="G31" s="32" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H31" s="11">
         <v>29</v>
@@ -2956,7 +2956,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K31" s="37" t="s">
         <v>30</v>
@@ -2967,7 +2967,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="17"/>
       <c r="O31" s="16" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P31" s="17" t="s">
         <v>29</v>
@@ -2982,7 +2982,7 @@
         <v>55</v>
       </c>
       <c r="T31" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="U31" s="20" t="s">
         <v>57</v>
@@ -3000,12 +3000,12 @@
         <v>49</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="23"/>
       <c r="G32" s="32" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H32" s="24">
         <v>30</v>
@@ -3014,7 +3014,7 @@
         <v>30</v>
       </c>
       <c r="J32" s="28" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K32" s="37" t="s">
         <v>30</v>
@@ -3025,7 +3025,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="17"/>
       <c r="O32" s="16" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="P32" s="17" t="s">
         <v>29</v>
@@ -3040,7 +3040,7 @@
         <v>55</v>
       </c>
       <c r="T32" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="U32" s="20" t="s">
         <v>57</v>
@@ -3058,7 +3058,7 @@
         <v>49</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="23"/>
@@ -3072,7 +3072,7 @@
         <v>30</v>
       </c>
       <c r="J33" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>30</v>
@@ -3104,7 +3104,7 @@
         <v>49</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="23"/>
@@ -3118,7 +3118,7 @@
         <v>30</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>29</v>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O34" s="16" t="s">
         <v>41</v>
@@ -3164,12 +3164,12 @@
         <v>49</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E35" s="34"/>
       <c r="F35" s="23"/>
       <c r="G35" s="27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H35" s="11">
         <v>33</v>
@@ -3186,10 +3186,10 @@
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P35" s="17" t="s">
         <v>30</v>
@@ -3204,7 +3204,7 @@
         <v>36</v>
       </c>
       <c r="T35" s="25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U35" s="20" t="s">
         <v>37</v>
@@ -3227,12 +3227,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -3247,6 +3241,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V10">

</xml_diff>

<commit_message>
Fórmula tema 11 y ajuste escaleta tema 08
Fórmula y escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/Escaleta_MA_06_08_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion08/Escaleta_MA_06_08_CO.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14320"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -830,6 +830,39 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -838,39 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1214,82 +1214,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="47"/>
+      <c r="N1" s="44"/>
       <c r="O1" s="38" t="s">
         <v>27</v>
       </c>
       <c r="P1" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="50" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1298,11 +1298,11 @@
       </c>
       <c r="O2" s="38"/>
       <c r="P2" s="38"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="39"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="50"/>
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
@@ -3227,6 +3227,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -3241,12 +3247,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V10">

</xml_diff>